<commit_message>
Replace temp.xlsx with more data
</commit_message>
<xml_diff>
--- a/data/temp.xlsx
+++ b/data/temp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yijin\Documents\Jin\Princeton\Academics\2024 Fall\COS436\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yubimamiya/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63FD71A-2E56-4F2E-BB1D-77576A9FB670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37A288E7-6591-7043-8953-ACE7339DFC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="8625" windowHeight="10643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="23100" windowHeight="14200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>None</t>
   </si>
@@ -361,19 +361,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -381,7 +381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>45554</v>
       </c>
@@ -389,7 +389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>45555</v>
       </c>
@@ -397,7 +397,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>45556</v>
       </c>
@@ -405,7 +405,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>45557</v>
       </c>
@@ -413,7 +413,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>45558</v>
       </c>
@@ -421,7 +421,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>45559</v>
       </c>
@@ -429,7 +429,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>45560</v>
       </c>
@@ -437,7 +437,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>45561</v>
       </c>
@@ -445,7 +445,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>45562</v>
       </c>
@@ -453,7 +453,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>45563</v>
       </c>
@@ -461,7 +461,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>45564</v>
       </c>
@@ -469,12 +469,196 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>45565</v>
       </c>
       <c r="B13">
         <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>45566</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>45567</v>
+      </c>
+      <c r="B15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>45568</v>
+      </c>
+      <c r="B16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>45569</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>45570</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>45571</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>45572</v>
+      </c>
+      <c r="B20">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>45573</v>
+      </c>
+      <c r="B21">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>45574</v>
+      </c>
+      <c r="B22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>45575</v>
+      </c>
+      <c r="B23">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>45576</v>
+      </c>
+      <c r="B24">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>45577</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>45578</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>45579</v>
+      </c>
+      <c r="B27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>45580</v>
+      </c>
+      <c r="B28">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>45581</v>
+      </c>
+      <c r="B29">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>45582</v>
+      </c>
+      <c r="B30">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>45583</v>
+      </c>
+      <c r="B31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>45584</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>45585</v>
+      </c>
+      <c r="B33">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>45586</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>45587</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>45588</v>
+      </c>
+      <c r="B36">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>